<commit_message>
Changes in column in excel file
</commit_message>
<xml_diff>
--- a/Europa.xlsx
+++ b/Europa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,168 +459,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D12"/>
+  <dimension ref="C2:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>500</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>300</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1">
         <v>200</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>400</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>450</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
         <v>500</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>100</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E10" s="1">
         <v>100</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>100</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E12" s="1">
         <v>200</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>9</v>
       </c>
     </row>
@@ -634,7 +634,7 @@
   <dimension ref="C4:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0D3379-B8E6-4C36-B940-8289AE12F99F}">
   <dimension ref="F8:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>